<commit_message>
Resolved perceived problem in Main
stdin did not like string literals with quotation marks. Tested mainCheck and mainEval successfully. Need to flesh out better terms, especially a recursor. Need to leave early for anniversary.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-20june2016.xlsx
+++ b/time-labor/week-of-20june2016.xlsx
@@ -38,6 +38,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -610,16 +612,16 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -836,12 +838,14 @@
       <c r="C13" s="19" t="n">
         <v>0.583333333333333</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="20" t="n">
+        <v>0.854166666666667</v>
+      </c>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="21" t="n">
         <f aca="false">IF((((D13-C13)+(F13-E13))*24)&gt;8,8,((D13-C13)+(F13-E13))*24)</f>
-        <v>-14</v>
+        <v>6.50000000000001</v>
       </c>
       <c r="H13" s="21" t="n">
         <f aca="false">IF(((D13-C13)+(F13-E13))*24&gt;8,((D13-C13)+(F13-E13))*24-8,0)</f>
@@ -856,13 +860,17 @@
       <c r="B14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19" t="n">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="D14" s="20" t="n">
+        <v>0.645833333333333</v>
+      </c>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21" t="n">
         <f aca="false">IF((((D14-C14)+(F14-E14))*24)&gt;8,8,((D14-C14)+(F14-E14))*24)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="21" t="n">
         <f aca="false">IF(((D14-C14)+(F14-E14))*24&gt;8,((D14-C14)+(F14-E14))*24-8,0)</f>
@@ -993,7 +1001,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>-14</v>
+        <v>10.5</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1037,7 +1045,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>-140</v>
+        <v>105</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1053,7 +1061,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>-140</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Reverted typePres', added test terms, beta redux working?
Evaluator seems to working on a beta redux! Running into a stack overflow when testing typePres.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-20june2016.xlsx
+++ b/time-labor/week-of-20june2016.xlsx
@@ -40,6 +40,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -138,9 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">// Multiple time entries on Friday carried onto Sunday to account for clocking out for seminar</t>
   </si>
   <si>
     <t xml:space="preserve">Sunday</t>
@@ -612,16 +612,16 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -885,13 +885,17 @@
       <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="19" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D15" s="20" t="n">
+        <v>0.833333333333333</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
         <f aca="false">IF((((D15-C15)+(F15-E15))*24)&gt;8,8,((D15-C15)+(F15-E15))*24)</f>
-        <v>0</v>
+        <v>6.99999999999999</v>
       </c>
       <c r="H15" s="21" t="n">
         <f aca="false">IF(((D15-C15)+(F15-E15))*24&gt;8,((D15-C15)+(F15-E15))*24-8,0)</f>
@@ -927,13 +931,17 @@
       <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.666666666666667</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -963,13 +971,10 @@
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
-      <c r="L18" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="19" t="n">
         <v>0</v>
@@ -997,11 +1002,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>10.5</v>
+        <v>19.5</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1023,7 +1028,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1045,7 +1050,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1061,7 +1066,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>105</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1090,14 +1095,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1110,14 +1115,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal entries and hours
A few more test terms to construct.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-20june2016.xlsx
+++ b/time-labor/week-of-20june2016.xlsx
@@ -43,6 +43,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -612,16 +613,16 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="7.1530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -956,13 +957,17 @@
       <c r="B18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="19" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>0.5625</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>0.500000000000001</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -1006,7 +1011,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>19.5</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1050,7 +1055,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1066,7 +1071,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>